<commit_message>
feat: Add initial IGU recovery analysis application, including interactive prompts, scenario logic, and data files.
</commit_message>
<xml_diff>
--- a/data/saint_gobain/saint gobain product database.xlsx
+++ b/data/saint_gobain/saint gobain product database.xlsx
@@ -7,14 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="DB" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="68">
+  <si>
+    <t>Group/ID</t>
+  </si>
   <si>
     <t>win_name</t>
   </si>
@@ -67,111 +70,163 @@
     <t>Desiccant</t>
   </si>
   <si>
-    <t>Group/ID</t>
+    <t>1. ORIGINAL COATINGS 100% AIR</t>
+  </si>
+  <si>
+    <t>2. ORIGINAL COATINGS 90% ARGON</t>
+  </si>
+  <si>
+    <t>3. DETERIORATED COATINGS 100% AIR</t>
+  </si>
+  <si>
+    <t>4. ORIGINAL COATINGS 66% ARGON</t>
+  </si>
+  <si>
+    <t>5. DETERIORATED COATINGS 66% ARGON</t>
+  </si>
+  <si>
+    <t>6. NEW</t>
   </si>
   <si>
     <t>1.1_DGU_6_16_6_Bronze</t>
   </si>
   <si>
+    <t>1.2_DGU_44.2_16_6_Bronze</t>
+  </si>
+  <si>
+    <t>1.3_TGU_6_16_6_16_6_Bronze_Low-e</t>
+  </si>
+  <si>
+    <t>2.1_DGU_6_16_6_Bronze</t>
+  </si>
+  <si>
+    <t>2.2_DGU_44.2_16_6_Bronze</t>
+  </si>
+  <si>
+    <t>2.3_DGU_6_16_6_16_6_Bronze_Low-e</t>
+  </si>
+  <si>
+    <t>3.1_DGU_6_16_6</t>
+  </si>
+  <si>
+    <t>3.2_DGU_44.2_16_6</t>
+  </si>
+  <si>
+    <t>3.3_TGU_6_16_6_16_6</t>
+  </si>
+  <si>
+    <t>4.1_DGU_6_16_6_Bronze</t>
+  </si>
+  <si>
+    <t>4.2_DGU_44.2_16_6_Bronze</t>
+  </si>
+  <si>
+    <t>4.3_TGU_6_16_6_16_6_Bronze_Low-e</t>
+  </si>
+  <si>
+    <t>5.1_DGU_6_16_6</t>
+  </si>
+  <si>
+    <t>5.2_DGU_44.2_16_6</t>
+  </si>
+  <si>
+    <t>5.3_TGU_6_16_6_16_6</t>
+  </si>
+  <si>
+    <t>6.1_DGU_6_16_6_Cool-Lite Xtreme 70 33</t>
+  </si>
+  <si>
+    <t>6.2_DGU_44.2_16_6_Cool-Lite Xtreme 70 33</t>
+  </si>
+  <si>
+    <t>6.3_TGU_6_16_6_16_6_Cool-Lite Xtreme 70 33_ECLAZ</t>
+  </si>
+  <si>
     <t>Facade</t>
   </si>
   <si>
     <t>Double</t>
   </si>
   <si>
+    <t>Triple</t>
+  </si>
+  <si>
+    <t>Triple glazing</t>
+  </si>
+  <si>
     <t>DGU 6 | 16 | 6 mm</t>
   </si>
   <si>
+    <t>DGU 44.2 | 16 | 6 mm</t>
+  </si>
+  <si>
+    <t>TGU 6 | 16 | 6 | 16 | 6 mm</t>
+  </si>
+  <si>
     <t>Planilux</t>
   </si>
   <si>
+    <t>PLANICLE</t>
+  </si>
+  <si>
+    <t>PLANICLE AR</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
+    <t>44.2 laminated glass on outside</t>
+  </si>
+  <si>
     <t>Annealed</t>
   </si>
   <si>
     <t>100% Air</t>
   </si>
   <si>
+    <t>90% Argon</t>
+  </si>
+  <si>
+    <t>66% Argon</t>
+  </si>
+  <si>
     <t>Aluminum</t>
   </si>
   <si>
+    <t>Swisspacer (Hybrid warm edge)</t>
+  </si>
+  <si>
     <t>SGG Reflectasol Bronze 6mm</t>
   </si>
   <si>
+    <t>SGG Reflectasol Bronze 4mm</t>
+  </si>
+  <si>
+    <t>Cool-Lite Xtreme 70/33</t>
+  </si>
+  <si>
+    <t>PLANITHERM FUTUR N 6mm SGG</t>
+  </si>
+  <si>
+    <t>PLANITHERM FUTUR N</t>
+  </si>
+  <si>
+    <t>ECLAZ</t>
+  </si>
+  <si>
     <t>Silicone</t>
   </si>
   <si>
     <t>Standard market</t>
-  </si>
-  <si>
-    <t>1.2_DGU_44.2_16_6_Bronze</t>
-  </si>
-  <si>
-    <t>DGU 44.2 | 16 | 6 mm</t>
-  </si>
-  <si>
-    <t>44.2 laminated glass on outside</t>
-  </si>
-  <si>
-    <t>1.3_TGU_6_16_6_16_6_Bronze_Low-e</t>
-  </si>
-  <si>
-    <t>Triple</t>
-  </si>
-  <si>
-    <t>TGU 6 | 16 | 6 | 16 | 6 mm</t>
-  </si>
-  <si>
-    <t>PLANITHERM FUTUR N 6mm SGG</t>
-  </si>
-  <si>
-    <t>1. ORIGINAL COATINGS 100% AIR</t>
-  </si>
-  <si>
-    <t>2.1_DGU_6_16_6_Bronze</t>
-  </si>
-  <si>
-    <t>90% Argon</t>
-  </si>
-  <si>
-    <t>2.2_DGU_44.2_16_6_Bronze</t>
-  </si>
-  <si>
-    <t>2.3_DGU_6_16_6_16_6_Bronze_Low-e</t>
-  </si>
-  <si>
-    <t>2. ORIGINAL COATINGS 90% ARGON</t>
-  </si>
-  <si>
-    <t>3.1_DGU_6_16_6</t>
-  </si>
-  <si>
-    <t>3.2_DGU_44.2_16_6</t>
-  </si>
-  <si>
-    <t>3.3_TGU_6_16_6_16_6</t>
-  </si>
-  <si>
-    <t>3. DETERIORATED COATINGS 100% AIR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -186,18 +241,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -227,13 +276,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,80 +575,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="17" width="15.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
+      <c r="A2" t="s">
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>2.983</v>
@@ -617,46 +657,45 @@
         <v>0.352</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="M2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s">
-        <v>30</v>
       </c>
       <c r="C3">
         <v>2.983</v>
@@ -671,46 +710,45 @@
         <v>0.317</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-      <c r="O3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="2"/>
-      <c r="B4" t="s">
-        <v>33</v>
       </c>
       <c r="C4">
         <v>1.736</v>
@@ -725,48 +763,48 @@
         <v>0.433</v>
       </c>
       <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="P4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
       </c>
       <c r="C5">
         <v>2.886</v>
@@ -781,46 +819,45 @@
         <v>0.353</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="M5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="Q5" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="R5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="2"/>
-      <c r="B6" t="s">
-        <v>40</v>
       </c>
       <c r="C6">
         <v>2.851</v>
@@ -835,46 +872,45 @@
         <v>0.319</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="Q6" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="R6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="B7" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="2"/>
-      <c r="B7" t="s">
-        <v>41</v>
       </c>
       <c r="C7">
         <v>1.609</v>
@@ -889,48 +925,48 @@
         <v>0.443</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="P7" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="Q7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="R7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="2" t="s">
-        <v>46</v>
+      <c r="A8" t="s">
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>2.983</v>
@@ -945,46 +981,45 @@
         <v>0.966</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="M8" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="O8" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="Q8" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="R8" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>2.928</v>
@@ -999,46 +1034,45 @@
         <v>1.011</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="B10" t="s">
         <v>32</v>
-      </c>
-      <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="2"/>
-      <c r="B10" t="s">
-        <v>45</v>
       </c>
       <c r="C10">
         <v>2.234</v>
@@ -1053,48 +1087,529 @@
         <v>0.967</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>66</v>
+      </c>
+      <c r="R10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>2.912</v>
+      </c>
+      <c r="D11">
+        <v>0.385</v>
+      </c>
+      <c r="E11">
+        <v>0.136</v>
+      </c>
+      <c r="F11">
+        <v>0.353</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>66</v>
+      </c>
+      <c r="R11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="I10" t="s">
+      <c r="C12">
+        <v>2.875</v>
+      </c>
+      <c r="D12">
+        <v>0.427</v>
+      </c>
+      <c r="E12">
+        <v>0.136</v>
+      </c>
+      <c r="F12">
+        <v>0.319</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>66</v>
+      </c>
+      <c r="R12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="J10" t="s">
+      <c r="C13">
+        <v>1.643</v>
+      </c>
+      <c r="D13">
+        <v>0.273</v>
+      </c>
+      <c r="E13">
+        <v>0.12</v>
+      </c>
+      <c r="F13">
+        <v>0.44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" t="s">
+        <v>60</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>66</v>
+      </c>
+      <c r="R13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="K10" t="s">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>2.912</v>
+      </c>
+      <c r="D14">
+        <v>0.715</v>
+      </c>
+      <c r="E14">
+        <v>0.891</v>
+      </c>
+      <c r="F14">
+        <v>0.966</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>66</v>
+      </c>
+      <c r="R14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>2.88</v>
+      </c>
+      <c r="D15">
+        <v>0.656</v>
+      </c>
+      <c r="E15">
+        <v>0.663</v>
+      </c>
+      <c r="F15">
+        <v>1.011</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" t="s">
+        <v>52</v>
+      </c>
+      <c r="P15" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>66</v>
+      </c>
+      <c r="R15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>2.178</v>
+      </c>
+      <c r="D16">
+        <v>0.645</v>
+      </c>
+      <c r="E16">
+        <v>0.624</v>
+      </c>
+      <c r="F16">
+        <v>0.967</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P16" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>66</v>
+      </c>
+      <c r="R16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s">
-        <v>23</v>
-      </c>
-      <c r="P10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" t="s">
-        <v>29</v>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17">
+        <v>1.116</v>
+      </c>
+      <c r="D17">
+        <v>0.28</v>
+      </c>
+      <c r="E17">
+        <v>0.599</v>
+      </c>
+      <c r="F17">
+        <v>2.139</v>
+      </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" t="s">
+        <v>59</v>
+      </c>
+      <c r="O17" t="s">
+        <v>62</v>
+      </c>
+      <c r="P17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1.118</v>
+      </c>
+      <c r="D18">
+        <v>0.28</v>
+      </c>
+      <c r="E18">
+        <v>0.603</v>
+      </c>
+      <c r="F18">
+        <v>2.154</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" t="s">
+        <v>59</v>
+      </c>
+      <c r="O18" t="s">
+        <v>62</v>
+      </c>
+      <c r="P18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>66</v>
+      </c>
+      <c r="R18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>0.726</v>
+      </c>
+      <c r="D19">
+        <v>0.253</v>
+      </c>
+      <c r="E19">
+        <v>0.55</v>
+      </c>
+      <c r="F19">
+        <v>2.174</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" t="s">
+        <v>54</v>
+      </c>
+      <c r="M19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" t="s">
+        <v>59</v>
+      </c>
+      <c r="O19" t="s">
+        <v>62</v>
+      </c>
+      <c r="P19" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>66</v>
+      </c>
+      <c r="R19" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>